<commit_message>
feature/004 - priprava release v1.2
</commit_message>
<xml_diff>
--- a/others/qa.xlsx
+++ b/others/qa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanBinder\OneDrive\Projects\sorryjako\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanBinder\Documents\sorryjako\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAA68D1-8361-40A2-8E95-027E9638D9B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055BD54-CDEF-4554-BA66-B1640948A883}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
   <si>
     <t>Product list</t>
   </si>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,111 +1039,177 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feature/004 - priprava release v1.2 (#15)
 feature/004 - priprava release v1.2
</commit_message>
<xml_diff>
--- a/others/qa.xlsx
+++ b/others/qa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanBinder\OneDrive\Projects\sorryjako\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanBinder\Documents\sorryjako\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAA68D1-8361-40A2-8E95-027E9638D9B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055BD54-CDEF-4554-BA66-B1640948A883}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
   <si>
     <t>Product list</t>
   </si>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,111 +1039,177 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feature/0020 - Release 1.3
</commit_message>
<xml_diff>
--- a/others/qa.xlsx
+++ b/others/qa.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanBinder\Documents\sorryjako\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055BD54-CDEF-4554-BA66-B1640948A883}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24BDD10-5D38-46DA-A8D7-DFD0977F8D2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.0.0" sheetId="2" r:id="rId1"/>
     <sheet name="1.1.0" sheetId="3" r:id="rId2"/>
     <sheet name="1.1.1" sheetId="4" r:id="rId3"/>
     <sheet name="1.2" sheetId="5" r:id="rId4"/>
+    <sheet name="1.3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1015,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B27973-C829-4818-AB99-B9766FB70518}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,4 +1215,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07DDD1D-8466-4F28-99E5-194A347FF91D}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>